<commit_message>
#100DaysOfCode #Day03 #JS Added tooltip on click
</commit_message>
<xml_diff>
--- a/data/uberRides.xlsx
+++ b/data/uberRides.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\BerkeleyMIDS\projects\w209\assignment01_personalData\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC8DC53-532C-405A-B989-C00B2991EEE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F1A279-59EB-4B2F-883F-21FF11CE3ED4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D0AA94EF-41C0-44AD-B89D-588C10285674}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D0AA94EF-41C0-44AD-B89D-588C10285674}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1329,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D16B3B-98C8-4D5F-8560-CD14E6AF5377}">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4543,8 +4543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949C3C1B-B1AF-453E-87F6-ABEC7151B111}">
   <dimension ref="C1:V102"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>